<commit_message>
Add a comment in the CCTool-OO Schema generated files to specify the GA version. Update the Survey UI display to add colors. Modify survey verification to add in Comments column information when multiple values exist.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_add_verif_014_dc_tu.xlsx
+++ b/prj/src/templates/template_add_verif_014_dc_tu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4566A276-E141-49B1-8B44-B6674013EFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5A24F8-1736-4D2C-B0A3-1133F9CF0BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EF4511BD-DD2E-4664-8583-D8C3C13D2563}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Author</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Core CBTC Referential:</t>
-  </si>
-  <si>
-    <t>C_D470:</t>
   </si>
   <si>
     <t>Date:</t>
@@ -143,8 +140,8 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -152,11 +149,9 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -300,7 +295,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -314,15 +309,8 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -356,32 +344,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -407,6 +399,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -467,16 +469,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -877,10 +869,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A6:G30"/>
+  <dimension ref="A6:G29"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B13" sqref="B13:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,62 +898,62 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
+      <c r="B13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="19"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
     </row>
     <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="19"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="16"/>
     </row>
     <row r="18" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="19"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="16"/>
     </row>
     <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="19"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16"/>
     </row>
     <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="22"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" spans="2:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
@@ -994,9 +986,9 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
@@ -1017,31 +1009,24 @@
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="9"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="30"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="11"/>
+      <c r="D29" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1065,44 +1050,44 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.42578125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="49.7109375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" style="13" customWidth="1"/>
-    <col min="8" max="8" width="53" style="13" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="13"/>
+    <col min="1" max="1" width="30.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.42578125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="49.7109375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" style="10" customWidth="1"/>
+    <col min="8" max="8" width="53" style="10" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23"/>
-      <c r="B1" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="28" t="s">
+    <row r="1" spans="1:8" s="9" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21"/>
+      <c r="B1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="12" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="29"/>
+      <c r="H1" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="9" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:H2" xr:uid="{D8CA666F-C951-4E28-B85E-ED54F83BCF49}">
@@ -1118,25 +1103,27 @@
     <mergeCell ref="G1:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576 G1:G1048576">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
-      <formula xml:space="preserve"> "KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula xml:space="preserve"> "NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula xml:space="preserve"> "OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula xml:space="preserve"> "KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula xml:space="preserve"> "NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula xml:space="preserve"> "OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576 E1:E1048576">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula xml:space="preserve"> "KO"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1156,34 +1143,34 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.42578125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="49.7109375" style="12" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="12"/>
+    <col min="1" max="1" width="30.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.42578125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="49.7109375" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23"/>
-      <c r="B1" s="24" t="s">
+      <c r="A1" s="21"/>
+      <c r="B1" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>8</v>
+      <c r="F1" s="20" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:F2" xr:uid="{9DE04395-FA11-44AD-A84B-74BB607C46AB}">

</xml_diff>